<commit_message>
Completed Example 4 in Working With Blocks and code analysis for RB101/Lesson_5
</commit_message>
<xml_diff>
--- a/rb101_programming_foundations/lesson_5/notes/analyzing_code.xlsx
+++ b/rb101_programming_foundations/lesson_5/notes/analyzing_code.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Line</t>
   </si>
@@ -44,6 +44,9 @@
     <t>Is Return Value Used?</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>method call (map)</t>
   </si>
   <si>
@@ -96,6 +99,72 @@
   </si>
   <si>
     <t>Example 3</t>
+  </si>
+  <si>
+    <t>Example 4</t>
+  </si>
+  <si>
+    <t>Note: Convert to markdown once finished</t>
+  </si>
+  <si>
+    <t>Variable assignment (my_arr)</t>
+  </si>
+  <si>
+    <t>1 thru 7</t>
+  </si>
+  <si>
+    <t>method call (each)</t>
+  </si>
+  <si>
+    <t>Yes, assigned to the variable `my_arr`</t>
+  </si>
+  <si>
+    <t>2 thru 6</t>
+  </si>
+  <si>
+    <t>Nil, if num &gt; 5 else num</t>
+  </si>
+  <si>
+    <t>outer block execution</t>
+  </si>
+  <si>
+    <t>inner block execution</t>
+  </si>
+  <si>
+    <t>[[18, 7],  [3, 12]]</t>
+  </si>
+  <si>
+    <t>Original array (calling object) [[18, 7], [3, 12]]</t>
+  </si>
+  <si>
+    <t>Each sub-array</t>
+  </si>
+  <si>
+    <t>The calling object: current sub-array</t>
+  </si>
+  <si>
+    <t>Yes, used to determine return value of outer block</t>
+  </si>
+  <si>
+    <t>3 thru 5</t>
+  </si>
+  <si>
+    <t>Conditional `if`</t>
+  </si>
+  <si>
+    <t>Comparison `&gt;`</t>
+  </si>
+  <si>
+    <t>Element of the sub array in that iteration</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Yes, to evaluate `if`</t>
+  </si>
+  <si>
+    <t>Yes, to determine return value of inner block</t>
   </si>
 </sst>
 </file>
@@ -137,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +219,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,186 +500,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="38.5" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="38.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" s="2">
-        <v>2</v>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A10:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed notes on Working with Blocks in RB101/Lesson_5
</commit_message>
<xml_diff>
--- a/rb101_programming_foundations/lesson_5/notes/analyzing_code.xlsx
+++ b/rb101_programming_foundations/lesson_5/notes/analyzing_code.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8520" windowWidth="28800" windowHeight="8960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="7360" windowWidth="28800" windowHeight="10100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
   <si>
     <t>Line</t>
   </si>
@@ -165,6 +165,48 @@
   </si>
   <si>
     <t>Yes, to determine return value of inner block</t>
+  </si>
+  <si>
+    <t>Example 5</t>
+  </si>
+  <si>
+    <t>Method call (map)</t>
+  </si>
+  <si>
+    <t>1 thru 5</t>
+  </si>
+  <si>
+    <t>Outer block execution</t>
+  </si>
+  <si>
+    <t>Yes, used to determine return value of inner block</t>
+  </si>
+  <si>
+    <t>New transformed array</t>
+  </si>
+  <si>
+    <t>2 thru 4</t>
+  </si>
+  <si>
+    <t>Inner block execution</t>
+  </si>
+  <si>
+    <t>Element of sub array in that iteration</t>
+  </si>
+  <si>
+    <t>Transformed element</t>
+  </si>
+  <si>
+    <t>num * 2</t>
+  </si>
+  <si>
+    <t>An integer</t>
+  </si>
+  <si>
+    <t>Yes, used by inner map for transformation</t>
+  </si>
+  <si>
+    <t>Yes, used by original map for transformation</t>
   </si>
 </sst>
 </file>
@@ -206,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,10 +260,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,12 +563,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -546,7 +591,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -567,7 +612,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -588,7 +633,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -609,7 +654,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -630,7 +675,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2">
         <v>3</v>
       </c>
@@ -651,7 +696,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -674,7 +719,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2">
         <v>1</v>
       </c>
@@ -695,7 +740,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2">
         <v>1</v>
       </c>
@@ -716,7 +761,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
@@ -737,7 +782,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2">
         <v>2</v>
       </c>
@@ -758,7 +803,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -779,7 +824,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2">
         <v>3</v>
       </c>
@@ -800,7 +845,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
@@ -821,7 +866,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="2">
         <v>4</v>
       </c>
@@ -841,10 +886,148 @@
         <v>46</v>
       </c>
     </row>
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A10:A18"/>
+    <mergeCell ref="A20:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>